<commit_message>
EPBDS-2852 test for custom spreadsheet result and testing spreadsheet
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/calc1/TestingSpreadsheet.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/calc1/TestingSpreadsheet.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
-    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
-    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
+    <sheet name="Spreadsheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Methods helpers" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Step</t>
   </si>
@@ -58,30 +58,6 @@
   </si>
   <si>
     <t>= coveredProperty + 1</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Spreadsheet SpreadsheetResult </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">test </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>(String coverageId, int coveredProperty, double koef)</t>
-    </r>
   </si>
   <si>
     <t>= koef * $Formula$Covered_Property</t>
@@ -128,26 +104,59 @@
     <t>$Formula$Final_Premium</t>
   </si>
   <si>
-    <t>//Testmethod method4Test testing</t>
-  </si>
-  <si>
     <t>Method DoubleValue method4Test1(String coverageId, int coveredProperty, double koef)</t>
   </si>
   <si>
     <t>Testmethod method4Test1 testing1</t>
   </si>
   <si>
-    <t>return test (coverageId, coveredProperty, koef).$formula$Final_Premium;</t>
-  </si>
-  <si>
     <t>$Text$Coverage_Id</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult test (String coverageId, int coveredProperty, double koef)</t>
+  </si>
+  <si>
+    <t>DoubleValue fp = test (coverageId, coveredProperty, koef).$Formula$Final_Premium;
+return fp;</t>
+  </si>
+  <si>
+    <t>Coverageid</t>
+  </si>
+  <si>
+    <t>Coveredproperty</t>
+  </si>
+  <si>
+    <t>Koef</t>
+  </si>
+  <si>
+    <t>Testmethod method4Test method4TestTest</t>
+  </si>
+  <si>
+    <t>cov1</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Method DoubleValue method4Test2(String coverageId, int coveredProperty, double koef)</t>
+  </si>
+  <si>
+    <t>SpreadsheetResulttest result = test(coverageId,coveredProperty, koef);
+DoubleValue fp = result.$Formula$Final_Premium;
+return fp;</t>
+  </si>
+  <si>
+    <t>Testmethod method4Test2 testing2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,13 +187,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,18 +233,54 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="53"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="40"/>
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -258,48 +328,27 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -311,30 +360,65 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -637,294 +721,386 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C42" sqref="C42:F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="24.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="2" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="2:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="12">
-        <v>1.23</v>
-      </c>
-      <c r="E12" s="12">
-        <v>6.15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="12">
-        <v>1.23</v>
-      </c>
-      <c r="E19" s="12">
-        <v>6.15</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B25" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B41" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="12">
-        <v>1.23</v>
-      </c>
-      <c r="E44" s="12">
-        <v>6.15</v>
-      </c>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B9:F9"/>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B4:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B18:B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="81.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B5:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="24" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="30"/>
+      <c r="E7" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="34">
+        <v>1.23</v>
+      </c>
+      <c r="E8" s="35">
+        <v>6.15</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1.23</v>
+      </c>
+      <c r="E15" s="5">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="39"/>
+      <c r="D19" s="39"/>
+      <c r="E19" s="39"/>
+    </row>
+    <row r="20" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1.23</v>
+      </c>
+      <c r="E22" s="5">
+        <v>6.15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E29" s="18">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="17"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B19:E19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-2947 Generate setters fir Custom Spreadsheet Results. Use _res_ field for comparing CSR cells.
</commit_message>
<xml_diff>
--- a/DEV/trunk/org.openl.rules/test/rules/calc1/TestingSpreadsheet.xlsx
+++ b/DEV/trunk/org.openl.rules/test/rules/calc1/TestingSpreadsheet.xlsx
@@ -101,16 +101,10 @@
     <t>Testmethod test TestSpr</t>
   </si>
   <si>
-    <t>$Formula$Final_Premium</t>
-  </si>
-  <si>
     <t>Method DoubleValue method4Test1(String coverageId, int coveredProperty, double koef)</t>
   </si>
   <si>
     <t>Testmethod method4Test1 testing1</t>
-  </si>
-  <si>
-    <t>$Text$Coverage_Id</t>
   </si>
   <si>
     <t>Spreadsheet SpreadsheetResult test (String coverageId, int coveredProperty, double koef)</t>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>Testmethod method4Test2 testing2</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$Final_Premium</t>
+  </si>
+  <si>
+    <t>_res_.$Text$Coverage_Id</t>
   </si>
 </sst>
 </file>
@@ -739,7 +739,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="36" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
@@ -840,22 +840,22 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -869,7 +869,7 @@
   <dimension ref="B5:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:E19"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,10 +900,10 @@
         <v>23</v>
       </c>
       <c r="E6" s="33" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="F6" s="33" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
@@ -990,7 +990,7 @@
     <row r="18" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="39" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -1039,7 +1039,7 @@
     <row r="24" spans="2:5" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -1061,13 +1061,13 @@
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="23" t="s">
         <v>33</v>
-      </c>
-      <c r="C28" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>35</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>16</v>
@@ -1075,13 +1075,13 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="19" t="s">
         <v>37</v>
-      </c>
-      <c r="C29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>39</v>
       </c>
       <c r="E29" s="18">
         <v>16.5</v>

</xml_diff>